<commit_message>
ROADM_Type added to excel and methods
</commit_message>
<xml_diff>
--- a/Khuzestan Network/Nodes.xlsx
+++ b/Khuzestan Network/Nodes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
   <si>
     <t>ID</t>
   </si>
@@ -30,9 +30,6 @@
     <t>Location</t>
   </si>
   <si>
-    <t>Type</t>
-  </si>
-  <si>
     <t>AR1</t>
   </si>
   <si>
@@ -121,6 +118,12 @@
   </si>
   <si>
     <t>31.295746 , 48.640885</t>
+  </si>
+  <si>
+    <t>ROADM_Type</t>
+  </si>
+  <si>
+    <t>Directionless</t>
   </si>
 </sst>
 </file>
@@ -504,13 +507,14 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="13.77734375" customWidth="1"/>
     <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -524,7 +528,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -532,13 +536,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -546,13 +550,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -560,13 +564,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -574,13 +578,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -588,13 +592,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="1">
-        <v>1</v>
+        <v>22</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -602,13 +606,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1</v>
+        <v>23</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -616,13 +620,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1</v>
+        <v>24</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -630,13 +634,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1</v>
+        <v>25</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -644,13 +648,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="1">
-        <v>1</v>
+        <v>32</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -658,13 +662,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="1">
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -672,13 +676,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="1">
-        <v>1</v>
+        <v>27</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -686,13 +690,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="1">
-        <v>1</v>
+        <v>28</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -700,13 +704,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="1">
-        <v>1</v>
+        <v>29</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -714,13 +718,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="1">
-        <v>1</v>
+        <v>30</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -728,13 +732,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="1">
-        <v>1</v>
+        <v>31</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>